<commit_message>
Add excel_to_json tool and update monitor scripts for API limits
</commit_message>
<xml_diff>
--- a/monitor_xlsx/20260204.xlsx
+++ b/monitor_xlsx/20260204.xlsx
@@ -541,12 +541,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>4.27%</t>
+          <t>4.28%</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>-0.12%</t>
+          <t>+0.14%</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -567,12 +567,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>5107.3$</t>
+          <t>5034.4$</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>+4.15%</t>
+          <t>+2.67%</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -593,12 +593,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>31.54</t>
+          <t>31.57</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>-0.12%</t>
+          <t>-0.02%</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -619,12 +619,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>7966.33</t>
+          <t>7619.16</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>-2.07%</t>
+          <t>-4.36%</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -645,12 +645,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>17.81</t>
+          <t>18.64</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>-1.06%</t>
+          <t>+3.56%</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -709,18 +709,18 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>53.82億</t>
+          <t>58.21億</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>29.38億</t>
+          <t>30.26億</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>146.91億</t>
+          <t>151.3億</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
@@ -765,7 +765,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>157.78億</t>
+          <t>162.17億</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -813,28 +813,28 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>-24.38億</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>-4.34億</t>
+          <t>-4.08億</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>-21.68億</t>
+          <t>-20.38億</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>-18.43億</t>
+          <t>-18.19億</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>-368.52億</t>
+          <t>-363.83億</t>
         </is>
       </c>
     </row>
@@ -938,7 +938,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>29.38億</t>
+          <t>30.26億</t>
         </is>
       </c>
     </row>
@@ -950,7 +950,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>146.91億</t>
+          <t>151.3億</t>
         </is>
       </c>
     </row>
@@ -969,7 +969,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>-4.34億</t>
+          <t>-4.08億</t>
         </is>
       </c>
     </row>
@@ -981,7 +981,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>-21.68億</t>
+          <t>-20.38億</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>-18.43億</t>
+          <t>-18.19億</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>-368.52億</t>
+          <t>-363.83億</t>
         </is>
       </c>
     </row>
@@ -1237,9 +1237,15 @@
       <c r="J4" t="n">
         <v>14722</v>
       </c>
+      <c r="K4" t="n">
+        <v>7630</v>
+      </c>
       <c r="L4" t="n">
         <v>36987</v>
       </c>
+      <c r="M4" t="n">
+        <v>-4012076</v>
+      </c>
       <c r="N4" t="n">
         <v>-0.14</v>
       </c>
@@ -1255,10 +1261,10 @@
         <v>0.08</v>
       </c>
       <c r="R4" t="n">
-        <v>705379</v>
+        <v>137907000</v>
       </c>
       <c r="S4" t="n">
-        <v>0.01</v>
+        <v>0.99</v>
       </c>
       <c r="T4" t="n">
         <v>71.86</v>
@@ -1295,9 +1301,15 @@
       <c r="J5" t="n">
         <v>12005</v>
       </c>
+      <c r="K5" t="n">
+        <v>10516</v>
+      </c>
       <c r="L5" t="n">
         <v>47175</v>
       </c>
+      <c r="M5" t="n">
+        <v>-29673</v>
+      </c>
       <c r="O5" t="inlineStr">
         <is>
           <t>中性</t>
@@ -1310,7 +1322,7 @@
         <v>-5.41</v>
       </c>
       <c r="R5" t="n">
-        <v>466034</v>
+        <v>2003000</v>
       </c>
       <c r="S5" t="n">
         <v>14.01</v>
@@ -1362,9 +1374,15 @@
       <c r="J6" t="n">
         <v>43</v>
       </c>
+      <c r="K6" t="n">
+        <v>2821</v>
+      </c>
       <c r="L6" t="n">
         <v>13618</v>
       </c>
+      <c r="M6" t="n">
+        <v>-78691</v>
+      </c>
       <c r="N6" t="n">
         <v>0.83</v>
       </c>
@@ -1380,10 +1398,10 @@
         <v>5.66</v>
       </c>
       <c r="R6" t="n">
-        <v>463077</v>
+        <v>3409000</v>
       </c>
       <c r="S6" t="n">
-        <v>0.11</v>
+        <v>0.8</v>
       </c>
       <c r="T6" t="n">
         <v>937.3200000000001</v>
@@ -1415,7 +1433,7 @@
         <v>2.87</v>
       </c>
       <c r="E7" t="n">
-        <v>82827</v>
+        <v>82828</v>
       </c>
       <c r="F7" s="6" t="n">
         <v>9144</v>
@@ -1432,9 +1450,15 @@
       <c r="J7" t="n">
         <v>431</v>
       </c>
+      <c r="K7" t="n">
+        <v>83558</v>
+      </c>
       <c r="L7" t="n">
         <v>407516</v>
       </c>
+      <c r="M7" t="n">
+        <v>-1105334</v>
+      </c>
       <c r="N7" t="n">
         <v>-8.73</v>
       </c>
@@ -1450,10 +1474,10 @@
         <v>4.58</v>
       </c>
       <c r="R7" t="n">
-        <v>477280</v>
+        <v>176374918</v>
       </c>
       <c r="S7" t="n">
-        <v>0</v>
+        <v>0.68</v>
       </c>
       <c r="T7" t="n">
         <v>41.29</v>
@@ -1485,7 +1509,7 @@
         <v>-0.41</v>
       </c>
       <c r="E8" t="n">
-        <v>7328</v>
+        <v>7342</v>
       </c>
       <c r="F8" s="6" t="n">
         <v>1112</v>
@@ -1502,9 +1526,15 @@
       <c r="J8" t="n">
         <v>169</v>
       </c>
+      <c r="K8" t="n">
+        <v>6152</v>
+      </c>
       <c r="L8" t="n">
         <v>32845</v>
       </c>
+      <c r="M8" t="n">
+        <v>-648628</v>
+      </c>
       <c r="N8" t="n">
         <v>-1.55</v>
       </c>
@@ -1520,10 +1550,10 @@
         <v>-2.92</v>
       </c>
       <c r="R8" t="n">
-        <v>542401</v>
+        <v>2200680</v>
       </c>
       <c r="S8" t="n">
-        <v>0.04</v>
+        <v>0.18</v>
       </c>
       <c r="T8" t="n">
         <v>1159.85</v>
@@ -1555,7 +1585,7 @@
         <v>-0.83</v>
       </c>
       <c r="E9" t="n">
-        <v>28787</v>
+        <v>29087</v>
       </c>
       <c r="F9" s="7" t="n">
         <v>-9645</v>
@@ -1564,7 +1594,7 @@
         <v>-27402</v>
       </c>
       <c r="H9" t="n">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="I9" t="n">
         <v>4257</v>
@@ -1572,9 +1602,15 @@
       <c r="J9" t="n">
         <v>203</v>
       </c>
+      <c r="K9" t="n">
+        <v>22274</v>
+      </c>
       <c r="L9" t="n">
         <v>103004</v>
       </c>
+      <c r="M9" t="n">
+        <v>-6482877</v>
+      </c>
       <c r="N9" t="n">
         <v>-0.45</v>
       </c>
@@ -1590,13 +1626,13 @@
         <v>9.210000000000001</v>
       </c>
       <c r="R9" t="n">
-        <v>297516</v>
+        <v>1556680</v>
       </c>
       <c r="S9" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="T9" t="n">
-        <v>1746.74</v>
+        <v>1746.76</v>
       </c>
       <c r="U9" t="n">
         <v>2.19</v>
@@ -1625,7 +1661,7 @@
         <v>2.84</v>
       </c>
       <c r="E10" t="n">
-        <v>210453</v>
+        <v>210454</v>
       </c>
       <c r="F10" s="6" t="n">
         <v>9060</v>
@@ -1642,9 +1678,15 @@
       <c r="J10" t="n">
         <v>1225</v>
       </c>
+      <c r="K10" t="n">
+        <v>143776</v>
+      </c>
       <c r="L10" t="n">
         <v>737181</v>
       </c>
+      <c r="M10" t="n">
+        <v>-1110204</v>
+      </c>
       <c r="N10" t="n">
         <v>-10.63</v>
       </c>
@@ -1660,10 +1702,10 @@
         <v>-0.99</v>
       </c>
       <c r="R10" t="n">
-        <v>77448</v>
+        <v>31176000</v>
       </c>
       <c r="S10" t="n">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="T10" t="n">
         <v>115.61</v>
@@ -1695,7 +1737,7 @@
         <v>9.970000000000001</v>
       </c>
       <c r="E11" t="n">
-        <v>6197</v>
+        <v>6355</v>
       </c>
       <c r="F11" s="6" t="n">
         <v>1067</v>
@@ -1712,9 +1754,15 @@
       <c r="J11" t="n">
         <v>272</v>
       </c>
+      <c r="K11" t="n">
+        <v>2160</v>
+      </c>
       <c r="L11" t="n">
         <v>10070</v>
       </c>
+      <c r="M11" t="n">
+        <v>-89471</v>
+      </c>
       <c r="N11" t="n">
         <v>12.4</v>
       </c>
@@ -1730,16 +1778,16 @@
         <v>-6.23</v>
       </c>
       <c r="R11" t="n">
-        <v>284917</v>
+        <v>1811528</v>
       </c>
       <c r="S11" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.45</v>
       </c>
       <c r="T11" t="n">
-        <v>1714.46</v>
+        <v>1714.99</v>
       </c>
       <c r="U11" t="n">
-        <v>18.99</v>
+        <v>18.95</v>
       </c>
       <c r="V11" t="inlineStr">
         <is>
@@ -1765,7 +1813,7 @@
         <v>1.96</v>
       </c>
       <c r="E12" t="n">
-        <v>2251</v>
+        <v>2252</v>
       </c>
       <c r="F12" s="6" t="n">
         <v>188</v>
@@ -1782,9 +1830,15 @@
       <c r="J12" t="n">
         <v>89</v>
       </c>
+      <c r="K12" t="n">
+        <v>5915</v>
+      </c>
       <c r="L12" t="n">
         <v>29768</v>
       </c>
+      <c r="M12" t="n">
+        <v>-19723</v>
+      </c>
       <c r="N12" t="n">
         <v>4.31</v>
       </c>
@@ -1800,10 +1854,10 @@
         <v>1.81</v>
       </c>
       <c r="R12" t="n">
-        <v>226892</v>
+        <v>5442503</v>
       </c>
       <c r="S12" t="n">
-        <v>0.1</v>
+        <v>2.38</v>
       </c>
       <c r="T12" t="n">
         <v>3400.14</v>
@@ -1852,9 +1906,15 @@
       <c r="J13" t="n">
         <v>1511</v>
       </c>
+      <c r="K13" t="n">
+        <v>28536</v>
+      </c>
       <c r="L13" t="n">
         <v>154614</v>
       </c>
+      <c r="M13" t="n">
+        <v>-267204</v>
+      </c>
       <c r="N13" t="n">
         <v>8.800000000000001</v>
       </c>
@@ -1870,10 +1930,10 @@
         <v>8.52</v>
       </c>
       <c r="R13" t="n">
-        <v>892315</v>
+        <v>22195945</v>
       </c>
       <c r="S13" t="n">
-        <v>0.02</v>
+        <v>0.44</v>
       </c>
       <c r="T13" t="n">
         <v>176.29</v>
@@ -1914,7 +1974,7 @@
         <v>2826</v>
       </c>
       <c r="H14" t="n">
-        <v>-76</v>
+        <v>17</v>
       </c>
       <c r="I14" t="n">
         <v>-82</v>
@@ -1922,9 +1982,15 @@
       <c r="J14" t="n">
         <v>6</v>
       </c>
+      <c r="K14" t="n">
+        <v>4429</v>
+      </c>
       <c r="L14" t="n">
         <v>22736</v>
       </c>
+      <c r="M14" t="n">
+        <v>-19211</v>
+      </c>
       <c r="N14" t="n">
         <v>7.89</v>
       </c>
@@ -1940,10 +2006,10 @@
         <v>-2.17</v>
       </c>
       <c r="R14" t="n">
-        <v>907512</v>
+        <v>1682000</v>
       </c>
       <c r="S14" t="n">
-        <v>0.18</v>
+        <v>0.33</v>
       </c>
       <c r="T14" t="n">
         <v>1475.92</v>
@@ -1992,9 +2058,15 @@
       <c r="J15" t="n">
         <v>19</v>
       </c>
+      <c r="K15" t="n">
+        <v>-50</v>
+      </c>
       <c r="L15" t="n">
         <v>-1493</v>
       </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
       <c r="N15" t="n">
         <v>0</v>
       </c>
@@ -2010,10 +2082,10 @@
         <v>9.31</v>
       </c>
       <c r="R15" t="n">
-        <v>96734</v>
+        <v>2188400</v>
       </c>
       <c r="S15" t="n">
-        <v>0.14</v>
+        <v>3.13</v>
       </c>
       <c r="T15" t="n">
         <v>775.1900000000001</v>
@@ -2062,9 +2134,15 @@
       <c r="J16" t="n">
         <v>457</v>
       </c>
+      <c r="K16" t="n">
+        <v>2454</v>
+      </c>
       <c r="L16" t="n">
         <v>-983</v>
       </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
       <c r="N16" t="n">
         <v>0</v>
       </c>
@@ -2080,10 +2158,10 @@
         <v>1.66</v>
       </c>
       <c r="R16" t="n">
-        <v>710486</v>
+        <v>8566640</v>
       </c>
       <c r="S16" t="n">
-        <v>0.04</v>
+        <v>0.45</v>
       </c>
       <c r="T16" t="n">
         <v>335.49</v>
@@ -2129,9 +2207,15 @@
       <c r="J17" t="n">
         <v>50</v>
       </c>
+      <c r="K17" t="n">
+        <v>22</v>
+      </c>
       <c r="L17" t="n">
         <v>-546</v>
       </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
       <c r="N17" t="n">
         <v>0</v>
       </c>
@@ -2147,10 +2231,10 @@
         <v>8.02</v>
       </c>
       <c r="R17" t="n">
-        <v>268088</v>
+        <v>1887000</v>
       </c>
       <c r="S17" t="n">
-        <v>0.28</v>
+        <v>1.94</v>
       </c>
       <c r="T17" t="n">
         <v>140.16</v>
@@ -2199,9 +2283,15 @@
       <c r="J18" t="n">
         <v>92</v>
       </c>
+      <c r="K18" t="n">
+        <v>198</v>
+      </c>
       <c r="L18" t="n">
         <v>-2547</v>
       </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
       <c r="N18" t="n">
         <v>0</v>
       </c>
@@ -2217,10 +2307,10 @@
         <v>-1.51</v>
       </c>
       <c r="R18" t="n">
-        <v>619737</v>
+        <v>11349993</v>
       </c>
       <c r="S18" t="n">
-        <v>0.03</v>
+        <v>0.55</v>
       </c>
       <c r="T18" t="n">
         <v>304.2</v>
@@ -2269,9 +2359,15 @@
       <c r="J19" t="n">
         <v>1540</v>
       </c>
+      <c r="K19" t="n">
+        <v>25655</v>
+      </c>
       <c r="L19" t="n">
         <v>153627</v>
       </c>
+      <c r="M19" t="n">
+        <v>-112769</v>
+      </c>
       <c r="N19" t="n">
         <v>11.73</v>
       </c>
@@ -2287,10 +2383,10 @@
         <v>-3.98</v>
       </c>
       <c r="R19" t="n">
-        <v>283932</v>
+        <v>10599826</v>
       </c>
       <c r="S19" t="n">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="T19" t="n">
         <v>216.26</v>

</xml_diff>